<commit_message>
Created ImgSeq.py, imshow3.py, and inputdlg2.py
</commit_message>
<xml_diff>
--- a/tests/tests_dir_mss0p/project_demo_test_output.xlsx
+++ b/tests/tests_dir_mss0p/project_demo_test_output.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="basic_info" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="camera_parameters" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="pois_definition" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="image_sources" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="basic_info" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pois_definition" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="image_sources" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="camera_parameters" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -471,729 +471,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>parameter_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>gopro7</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>gopro121</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>gopro122</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>image_width</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2704</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3840</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3840</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>image_height</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2028</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3360</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>3360</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>rvec_x</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.378853181077617</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.353109317968901</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0.628642883922084</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>rvec_y</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>-0.349687126135229</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-0.387044378764206</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>-0.00773758480014759</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>rvec_z</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.10072413733213</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>1.59595432439505</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>-0.0132550029751834</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>tvec_x</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>211.489660102207</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>353.961659529372</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>-314.458350442263</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>tvec_y</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>-52.2412973710651</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>55.5191012598572</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>55.7530794507648</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>tvec_z</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>-122.648043788326</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>-80.5381613907982</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>-39.6396935521477</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>cmat11_fx</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1046.72811993627</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1645.3487781477</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1988.30540933728</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>cmat12</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>cmat13_cx</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1272.39368044641</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1853.36635341203</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>1989.16985030597</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>cmat21</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>cmat22_fy</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1057.45622341859</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1671.89183909301</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>2081.77158859844</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>cmat23_cy</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>987.521814861355</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1609.17463112385</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>1627.15064102301</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>cmat31</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>cmat32</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>cmat33</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>k1</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>-0.146492861249863</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>-0.18214005131777</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>-0.265290395955887</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>k2</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>0.0135773895209156</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0.0222244255856692</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>0.0500182435490484</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>p1</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>p2</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>k3</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>k4</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>k5</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>k6</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>s1</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>s2</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>s3</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>s4</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>tau_x</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>tau_y</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2019,7 +1296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2084,4 +1361,541 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>parameters</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>gopro7</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>gopro121</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>gopro122</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>image_width</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2704</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3840</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>image_height</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2028</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3360</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>rvec_x</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.378853181077617</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.353109317968901</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.628642883922084</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rvec_y</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.349687126135229</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.387044378764206</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.00773758480014759</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rvec_z</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.10072413733213</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.59595432439505</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.0132550029751834</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tvec_x</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>211.489660102207</v>
+      </c>
+      <c r="C7" t="n">
+        <v>353.961659529372</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-314.458350442263</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>tvec_y</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-52.2412973710651</v>
+      </c>
+      <c r="C8" t="n">
+        <v>55.5191012598572</v>
+      </c>
+      <c r="D8" t="n">
+        <v>55.7530794507648</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>tvec_z</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-122.648043788326</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-80.53816139079819</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-39.6396935521477</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>cmat11_fx</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1046.72811993627</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1645.3487781477</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1988.30540933728</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>cmat12</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>cmat13_cx</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1272.39368044641</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1853.36635341203</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1989.16985030597</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cmat21</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>cmat22_fy</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1057.45622341859</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1671.89183909301</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2081.77158859844</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>cmat23_cy</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>987.521814861355</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1609.17463112385</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1627.15064102301</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>cmat31</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>cmat32</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>cmat33</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>k1</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-0.146492861249863</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.18214005131777</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.265290395955887</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>k2</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.0135773895209156</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0222244255856692</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.0500182435490484</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>p1</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>p2</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>k3</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>k4</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>k5</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>k6</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>s1</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>s2</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>s3</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>s4</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>tau_x</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>tau_y</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>